<commit_message>
Tune Linear Regression model.  Score: 9.02
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcwork/Desktop/Tabular Playground/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732C9116-E7F7-2747-9F7C-2EB8501632E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC57F250-2B27-0E47-A241-F8952498B41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1940" windowWidth="28040" windowHeight="16020" xr2:uid="{C8A5DF3F-15CA-424B-9AB6-8953FD2B902F}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="17800" windowHeight="13040" xr2:uid="{C8A5DF3F-15CA-424B-9AB6-8953FD2B902F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Tabular Playground Series - Jan 2022</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>All Features</t>
+  </si>
+  <si>
+    <t>Tuned</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904BB077-2FA1-CA48-837D-32985D1FADDC}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,6 +528,20 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>44582</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>9.02</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>

</xml_diff>